<commit_message>
Executed small problems folder
</commit_message>
<xml_diff>
--- a/BBDD.xlsx
+++ b/BBDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\googleMapsVS\Google-Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260F1C51-BC02-4A7C-BEA1-96B97CA4513C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BABE4C7-9668-4D68-8B7F-F8EDFB05B24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7F71742E-253B-424F-BD00-490871758625}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
   <si>
     <t>Problem</t>
   </si>
@@ -78,6 +78,21 @@
   </si>
   <si>
     <t>small</t>
+  </si>
+  <si>
+    <t>avenida_de_espanÌa_250_0.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avenida_de_espanÌa_250_1.json </t>
+  </si>
+  <si>
+    <t>avenida_de_espanÌa_250_1.json</t>
+  </si>
+  <si>
+    <t>paseo_simoÌn_abril_250_0.json</t>
+  </si>
+  <si>
+    <t>paseo_simoÌn_abril_250_1.json</t>
   </si>
 </sst>
 </file>
@@ -85,8 +100,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="171" formatCode="#,##0.00000"/>
-    <numFmt numFmtId="179" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -128,8 +143,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0067E397-AC89-489C-845E-5ACB9E66F72E}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,6 +625,178 @@
         <v>13</v>
       </c>
     </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>6.4625666666666604</v>
+      </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>4.2389333333333301</v>
+      </c>
+      <c r="G7">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <v>9</v>
+      </c>
+      <c r="F8">
+        <v>15.4287333333333</v>
+      </c>
+      <c r="G8">
+        <v>25</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>39</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>15.4287333333333</v>
+      </c>
+      <c r="G9">
+        <v>70</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>25</v>
+      </c>
+      <c r="D12">
+        <v>36</v>
+      </c>
+      <c r="E12">
+        <v>12</v>
+      </c>
+      <c r="F12">
+        <v>27.5196166666666</v>
+      </c>
+      <c r="G12">
+        <v>43</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <v>35</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <v>20.158433333333299</v>
+      </c>
+      <c r="G13">
+        <v>84</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>